<commit_message>
Commit for production after final checks and publication quality figures
</commit_message>
<xml_diff>
--- a/output/BayesDiscovCitptile0.9alpha0.05power0.8N1000/BayesDiscovCitptile0.9alpha0.05power0.8N1000N1000.xlsx
+++ b/output/BayesDiscovCitptile0.9alpha0.05power0.8N1000/BayesDiscovCitptile0.9alpha0.05power0.8N1000N1000.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lewan\Documents\MATLAB\Modeling\Replication market\output\BayesDiscovCitptile0.9alpha0.05power0.8N1000\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D03A8FF-1F7C-4B89-BF71-C606509F48F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C2D3C1-7E17-4E05-8E9F-59579FE7490C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29190" yWindow="2250" windowWidth="21600" windowHeight="12735" xr2:uid="{64EBE5A4-F879-4D30-94E8-A1EB52AC217C}"/>
+    <workbookView xWindow="1152" yWindow="6684" windowWidth="27060" windowHeight="10800" xr2:uid="{6351EA0B-012B-4E58-B511-738914952FE8}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="4" r:id="rId1"/>
@@ -466,29 +466,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFEECE58-6F21-43BE-B10A-B6865D7E8793}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52FCE626-424D-4B6A-9C4E-BFE7E761DB63}">
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -535,7 +535,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -543,46 +543,46 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1.5415115851045148E-2</v>
+        <v>1.4883962683362348E-2</v>
       </c>
       <c r="D2">
-        <v>0.9070697771764169</v>
+        <v>0.90352996582430845</v>
       </c>
       <c r="E2">
-        <v>9.0519999999999996</v>
+        <v>9.1289999999999996</v>
       </c>
       <c r="F2">
-        <v>109.499</v>
+        <v>109.551</v>
       </c>
       <c r="G2">
-        <v>7.3369999999999997</v>
+        <v>7.3769999999999998</v>
       </c>
       <c r="H2">
+        <v>1.07</v>
+      </c>
+      <c r="I2">
+        <v>1.0609999999999999</v>
+      </c>
+      <c r="J2">
+        <v>1.7535650623885915E-2</v>
+      </c>
+      <c r="K2">
+        <v>0.90141303388110494</v>
+      </c>
+      <c r="L2">
+        <v>9.5510000000000002</v>
+      </c>
+      <c r="M2">
+        <v>109.551</v>
+      </c>
+      <c r="N2">
         <v>1.0960000000000001</v>
       </c>
-      <c r="I2">
-        <v>1.171</v>
-      </c>
-      <c r="J2">
-        <v>1.6932270916334664E-2</v>
-      </c>
-      <c r="K2">
-        <v>0.9017879773505193</v>
-      </c>
-      <c r="L2">
-        <v>9.4990000000000006</v>
-      </c>
-      <c r="M2">
-        <v>109.499</v>
-      </c>
-      <c r="N2">
-        <v>1.1040000000000001</v>
-      </c>
       <c r="O2">
-        <v>0.97799999999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.0449999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -590,46 +590,46 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1.5955211121210719E-2</v>
+        <v>1.5174759235628376E-2</v>
       </c>
       <c r="D3">
-        <v>0.89887953165518486</v>
+        <v>0.90221318562387509</v>
       </c>
       <c r="E3">
-        <v>9.0399999999999991</v>
+        <v>9.0510000000000002</v>
       </c>
       <c r="F3">
-        <v>109.601</v>
+        <v>109.70699999999999</v>
       </c>
       <c r="G3">
-        <v>7.38</v>
+        <v>7.5460000000000003</v>
       </c>
       <c r="H3">
-        <v>0.69599999999999995</v>
+        <v>0.77700000000000002</v>
       </c>
       <c r="I3">
-        <v>0.75800000000000001</v>
+        <v>0.72</v>
       </c>
       <c r="J3">
-        <v>1.3888888888888888E-2</v>
+        <v>1.1904761904761904E-2</v>
       </c>
       <c r="K3">
-        <v>0.91081621004566227</v>
+        <v>0.90837773830669044</v>
       </c>
       <c r="L3">
-        <v>9.6010000000000009</v>
+        <v>9.7070000000000007</v>
       </c>
       <c r="M3">
-        <v>101.002</v>
+        <v>100.95099999999999</v>
       </c>
       <c r="N3">
-        <v>0.79100000000000004</v>
+        <v>0.76800000000000002</v>
       </c>
       <c r="O3">
-        <v>0.78400000000000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.76200000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -637,46 +637,46 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>1.6311681929233882E-2</v>
+        <v>1.5865319637310481E-2</v>
       </c>
       <c r="D4">
-        <v>0.90386476575603991</v>
+        <v>0.9007840923945124</v>
       </c>
       <c r="E4">
-        <v>9.1359999999999992</v>
+        <v>8.9920000000000009</v>
       </c>
       <c r="F4">
-        <v>109.804</v>
+        <v>109.46</v>
       </c>
       <c r="G4">
-        <v>7.5750000000000002</v>
+        <v>7.2380000000000004</v>
       </c>
       <c r="H4">
-        <v>1.139</v>
+        <v>1.0369999999999999</v>
       </c>
       <c r="I4">
-        <v>1.075</v>
+        <v>1.054</v>
       </c>
       <c r="J4">
-        <v>6.0679611650485436E-3</v>
+        <v>6.3157894736842104E-3</v>
       </c>
       <c r="K4">
-        <v>0.89728082512892626</v>
+        <v>0.8990599593495936</v>
       </c>
       <c r="L4">
-        <v>9.8040000000000003</v>
+        <v>9.4600000000000009</v>
       </c>
       <c r="M4">
-        <v>101.416</v>
+        <v>101.345</v>
       </c>
       <c r="N4">
-        <v>1.133</v>
+        <v>1.0329999999999999</v>
       </c>
       <c r="O4">
-        <v>1.1299999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
@@ -684,46 +684,46 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>1.5916010602135634E-2</v>
+        <v>1.5176748520107017E-2</v>
       </c>
       <c r="D5">
-        <v>0.89634059266668709</v>
+        <v>0.8987125758425546</v>
       </c>
       <c r="E5">
-        <v>9.0879999999999992</v>
+        <v>8.9760000000000009</v>
       </c>
       <c r="F5">
-        <v>109.508</v>
+        <v>109.526</v>
       </c>
       <c r="G5">
-        <v>7.2789999999999999</v>
+        <v>7.3449999999999998</v>
       </c>
       <c r="H5">
-        <v>1.75</v>
+        <v>1.7370000000000001</v>
       </c>
       <c r="I5">
-        <v>1.7809999999999999</v>
+        <v>1.74</v>
       </c>
       <c r="J5">
-        <v>6.1576354679802959E-3</v>
+        <v>1.2562814070351759E-2</v>
       </c>
       <c r="K5">
-        <v>0.89994433025008536</v>
+        <v>0.90559452523524331</v>
       </c>
       <c r="L5">
-        <v>9.5079999999999991</v>
+        <v>9.5259999999999998</v>
       </c>
       <c r="M5">
-        <v>102.245</v>
+        <v>102.224</v>
       </c>
       <c r="N5">
-        <v>1.726</v>
+        <v>1.73</v>
       </c>
       <c r="O5">
-        <v>1.7230000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.7250000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -731,46 +731,46 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>1.476624542602558E-2</v>
+        <v>1.596507014703364E-2</v>
       </c>
       <c r="D6">
-        <v>0.90603707745419226</v>
+        <v>0.90173982913468387</v>
       </c>
       <c r="E6">
-        <v>9.0259999999999998</v>
+        <v>9.0120000000000005</v>
       </c>
       <c r="F6">
-        <v>109.559</v>
+        <v>109.663</v>
       </c>
       <c r="G6">
-        <v>7.4459999999999997</v>
+        <v>7.4130000000000003</v>
       </c>
       <c r="H6">
-        <v>1.0669999999999999</v>
+        <v>1.0449999999999999</v>
       </c>
       <c r="I6">
-        <v>0.98699999999999999</v>
+        <v>1.1140000000000001</v>
       </c>
       <c r="J6">
-        <v>1.1822985468956406E-2</v>
+        <v>1.3445000641766141E-2</v>
       </c>
       <c r="K6">
-        <v>0.90359685134836254</v>
+        <v>0.90306812401370684</v>
       </c>
       <c r="L6">
-        <v>9.5589999999999993</v>
+        <v>9.6630000000000003</v>
       </c>
       <c r="M6">
-        <v>109.559</v>
+        <v>109.663</v>
       </c>
       <c r="N6">
+        <v>1.087</v>
+      </c>
+      <c r="O6">
         <v>1.0189999999999999</v>
       </c>
-      <c r="O6">
-        <v>1.0960000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -778,46 +778,46 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>1.5314205932982673E-2</v>
+        <v>1.537015562728467E-2</v>
       </c>
       <c r="D7">
-        <v>0.90575547132338274</v>
+        <v>0.90147767914664856</v>
       </c>
       <c r="E7">
-        <v>8.9939999999999998</v>
+        <v>9.0419999999999998</v>
       </c>
       <c r="F7">
-        <v>109.46299999999999</v>
+        <v>109.56</v>
       </c>
       <c r="G7">
-        <v>7.2539999999999996</v>
+        <v>7.4180000000000001</v>
       </c>
       <c r="H7">
-        <v>0.76700000000000002</v>
+        <v>0.78500000000000003</v>
       </c>
       <c r="I7">
-        <v>0.73099999999999998</v>
+        <v>0.72599999999999998</v>
       </c>
       <c r="J7">
-        <v>5.1229508196721308E-3</v>
+        <v>1.1387163561076604E-2</v>
       </c>
       <c r="K7">
-        <v>0.90381944444444473</v>
+        <v>0.89694348327566331</v>
       </c>
       <c r="L7">
-        <v>9.4629999999999992</v>
+        <v>9.56</v>
       </c>
       <c r="M7">
-        <v>100.95099999999999</v>
+        <v>100.95699999999999</v>
       </c>
       <c r="N7">
-        <v>0.76300000000000001</v>
+        <v>0.77700000000000002</v>
       </c>
       <c r="O7">
-        <v>0.76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.77100000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -825,46 +825,46 @@
         <v>5</v>
       </c>
       <c r="C8">
-        <v>1.5537489283347153E-2</v>
+        <v>1.4614581794426425E-2</v>
       </c>
       <c r="D8">
-        <v>0.89535830723139664</v>
+        <v>0.90131401203164729</v>
       </c>
       <c r="E8">
-        <v>9.2509999999999994</v>
+        <v>8.9719999999999995</v>
       </c>
       <c r="F8">
-        <v>109.517</v>
+        <v>109.393</v>
       </c>
       <c r="G8">
-        <v>7.3170000000000002</v>
+        <v>7.3010000000000002</v>
       </c>
       <c r="H8">
-        <v>1.028</v>
+        <v>1.0289999999999999</v>
       </c>
       <c r="I8">
-        <v>1.054</v>
+        <v>1.0820000000000001</v>
       </c>
       <c r="J8">
-        <v>1.8049155145929339E-2</v>
+        <v>2.1428571428571429E-2</v>
       </c>
       <c r="K8">
-        <v>0.90465577018325893</v>
+        <v>0.89617604617604607</v>
       </c>
       <c r="L8">
-        <v>9.5169999999999995</v>
+        <v>9.3930000000000007</v>
       </c>
       <c r="M8">
-        <v>101.32</v>
+        <v>101.363</v>
       </c>
       <c r="N8">
-        <v>1.038</v>
+        <v>1.089</v>
       </c>
       <c r="O8">
-        <v>1.0289999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.079</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -872,46 +872,46 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>1.516480411979524E-2</v>
+        <v>1.5513216488301781E-2</v>
       </c>
       <c r="D9">
-        <v>0.90898318203374284</v>
+        <v>0.90022497682052305</v>
       </c>
       <c r="E9">
-        <v>8.8510000000000009</v>
+        <v>9.0630000000000006</v>
       </c>
       <c r="F9">
-        <v>109.49299999999999</v>
+        <v>109.57299999999999</v>
       </c>
       <c r="G9">
-        <v>7.375</v>
+        <v>7.39</v>
       </c>
       <c r="H9">
-        <v>1.6519999999999999</v>
+        <v>1.704</v>
       </c>
       <c r="I9">
-        <v>1.7070000000000001</v>
+        <v>1.901</v>
       </c>
       <c r="J9">
-        <v>1.0840108401084011E-2</v>
+        <v>9.8280098280098278E-3</v>
       </c>
       <c r="K9">
-        <v>0.89928180192264684</v>
+        <v>0.90364327979712555</v>
       </c>
       <c r="L9">
-        <v>9.4930000000000003</v>
+        <v>9.5730000000000004</v>
       </c>
       <c r="M9">
-        <v>102.188</v>
+        <v>102.292</v>
       </c>
       <c r="N9">
-        <v>1.7130000000000001</v>
+        <v>1.764</v>
       </c>
       <c r="O9">
-        <v>1.708</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.7589999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5</v>
       </c>
@@ -919,46 +919,46 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>1.6383666202989984E-2</v>
+        <v>1.741302153736176E-2</v>
       </c>
       <c r="D10">
-        <v>0.8973101550513265</v>
+        <v>0.90654585766799423</v>
       </c>
       <c r="E10">
-        <v>9.1050000000000004</v>
+        <v>8.8800000000000008</v>
       </c>
       <c r="F10">
-        <v>109.637</v>
+        <v>109.46</v>
       </c>
       <c r="G10">
-        <v>7.37</v>
+        <v>7.1319999999999997</v>
       </c>
       <c r="H10">
-        <v>1.0429999999999999</v>
+        <v>1.0309999999999999</v>
       </c>
       <c r="I10">
-        <v>1.044</v>
+        <v>0.96299999999999997</v>
       </c>
       <c r="J10">
-        <v>1.0898254576415493E-2</v>
+        <v>2.2719734660033165E-2</v>
       </c>
       <c r="K10">
-        <v>0.89955957045029855</v>
+        <v>0.90553988503782112</v>
       </c>
       <c r="L10">
-        <v>9.6370000000000005</v>
+        <v>9.4600000000000009</v>
       </c>
       <c r="M10">
-        <v>109.637</v>
+        <v>109.46</v>
       </c>
       <c r="N10">
-        <v>1.032</v>
+        <v>1.075</v>
       </c>
       <c r="O10">
-        <v>1.0109999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.016</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>5</v>
       </c>
@@ -966,46 +966,46 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>1.6065906880420318E-2</v>
+        <v>1.6532862716187636E-2</v>
       </c>
       <c r="D11">
-        <v>0.90608658053936308</v>
+        <v>0.90985858288897004</v>
       </c>
       <c r="E11">
-        <v>8.9190000000000005</v>
+        <v>9.0839999999999996</v>
       </c>
       <c r="F11">
-        <v>109.563</v>
+        <v>109.706</v>
       </c>
       <c r="G11">
-        <v>7.3659999999999997</v>
+        <v>7.4370000000000003</v>
       </c>
       <c r="H11">
-        <v>0.78500000000000003</v>
+        <v>0.76700000000000002</v>
       </c>
       <c r="I11">
-        <v>0.749</v>
+        <v>0.69</v>
       </c>
       <c r="J11">
-        <v>2.446183953033268E-2</v>
+        <v>7.8125E-3</v>
       </c>
       <c r="K11">
-        <v>0.89774696707105717</v>
+        <v>0.90828985507246374</v>
       </c>
       <c r="L11">
-        <v>9.5630000000000006</v>
+        <v>9.7059999999999995</v>
       </c>
       <c r="M11">
-        <v>100.96599999999999</v>
+        <v>100.98</v>
       </c>
       <c r="N11">
-        <v>0.77600000000000002</v>
+        <v>0.77700000000000002</v>
       </c>
       <c r="O11">
-        <v>0.76300000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.77300000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>5</v>
       </c>
@@ -1013,46 +1013,46 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>1.7156574592210972E-2</v>
+        <v>1.6628701283128645E-2</v>
       </c>
       <c r="D12">
-        <v>0.90587730694099944</v>
+        <v>0.9088079194985782</v>
       </c>
       <c r="E12">
-        <v>9.1750000000000007</v>
+        <v>9.1869999999999994</v>
       </c>
       <c r="F12">
-        <v>109.91800000000001</v>
+        <v>109.789</v>
       </c>
       <c r="G12">
-        <v>7.673</v>
+        <v>7.4630000000000001</v>
       </c>
       <c r="H12">
-        <v>1.0669999999999999</v>
+        <v>1.137</v>
       </c>
       <c r="I12">
-        <v>1.0329999999999999</v>
+        <v>1.046</v>
       </c>
       <c r="J12">
-        <v>1.6203703703703703E-2</v>
+        <v>1.7647058823529412E-2</v>
       </c>
       <c r="K12">
-        <v>0.89186875891583439</v>
+        <v>0.90099715099715116</v>
       </c>
       <c r="L12">
-        <v>9.9179999999999993</v>
+        <v>9.7889999999999997</v>
       </c>
       <c r="M12">
-        <v>101.435</v>
+        <v>101.38</v>
       </c>
       <c r="N12">
-        <v>1.121</v>
+        <v>1.087</v>
       </c>
       <c r="O12">
-        <v>1.1140000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.079</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>5</v>
       </c>
@@ -1060,46 +1060,46 @@
         <v>10</v>
       </c>
       <c r="C13">
-        <v>1.6100449142958197E-2</v>
+        <v>1.7091245920255852E-2</v>
       </c>
       <c r="D13">
-        <v>0.89581498532186243</v>
+        <v>0.90848852605569674</v>
       </c>
       <c r="E13">
-        <v>8.9320000000000004</v>
+        <v>8.8989999999999991</v>
       </c>
       <c r="F13">
-        <v>109.458</v>
+        <v>109.55500000000001</v>
       </c>
       <c r="G13">
-        <v>7.2460000000000004</v>
+        <v>7.2889999999999997</v>
       </c>
       <c r="H13">
-        <v>1.61</v>
+        <v>1.536</v>
       </c>
       <c r="I13">
-        <v>1.7150000000000001</v>
+        <v>1.6679999999999999</v>
       </c>
       <c r="J13">
-        <v>1.8217054263565891E-2</v>
+        <v>2.2169437846397463E-2</v>
       </c>
       <c r="K13">
-        <v>0.90912412926801422</v>
+        <v>0.90525698260073229</v>
       </c>
       <c r="L13">
-        <v>9.4580000000000002</v>
+        <v>9.5549999999999997</v>
       </c>
       <c r="M13">
-        <v>102.312</v>
+        <v>102.259</v>
       </c>
       <c r="N13">
-        <v>1.772</v>
+        <v>1.7170000000000001</v>
       </c>
       <c r="O13">
-        <v>1.7629999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.7070000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10</v>
       </c>
@@ -1107,46 +1107,46 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <v>1.9142560399034142E-2</v>
+        <v>1.9394941785746855E-2</v>
       </c>
       <c r="D14">
-        <v>0.9182016216965958</v>
+        <v>0.91766703379609738</v>
       </c>
       <c r="E14">
-        <v>8.9480000000000004</v>
+        <v>8.9870000000000001</v>
       </c>
       <c r="F14">
-        <v>110.02800000000001</v>
+        <v>110.05200000000001</v>
       </c>
       <c r="G14">
-        <v>7.6070000000000002</v>
+        <v>7.6580000000000004</v>
       </c>
       <c r="H14">
-        <v>1.143</v>
+        <v>1.0469999999999999</v>
       </c>
       <c r="I14">
-        <v>1.1319999999999999</v>
+        <v>1.163</v>
       </c>
       <c r="J14">
-        <v>2.5159872102318147E-2</v>
+        <v>1.6487669053301512E-2</v>
       </c>
       <c r="K14">
-        <v>0.91577365381052345</v>
+        <v>0.91397982160994151</v>
       </c>
       <c r="L14">
-        <v>10.028</v>
+        <v>10.052</v>
       </c>
       <c r="M14">
-        <v>110.02800000000001</v>
+        <v>110.05200000000001</v>
       </c>
       <c r="N14">
-        <v>1.046</v>
+        <v>1.0880000000000001</v>
       </c>
       <c r="O14">
-        <v>1.171</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.173</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10</v>
       </c>
@@ -1154,46 +1154,46 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>1.8958340408901868E-2</v>
+        <v>2.0241627082254191E-2</v>
       </c>
       <c r="D15">
-        <v>0.91447616449242819</v>
+        <v>0.91833193443335603</v>
       </c>
       <c r="E15">
-        <v>8.91</v>
+        <v>9.1419999999999995</v>
       </c>
       <c r="F15">
-        <v>109.916</v>
+        <v>110.28700000000001</v>
       </c>
       <c r="G15">
-        <v>7.5739999999999998</v>
+        <v>7.7939999999999996</v>
       </c>
       <c r="H15">
-        <v>0.76800000000000002</v>
+        <v>0.84199999999999997</v>
       </c>
       <c r="I15">
-        <v>0.748</v>
+        <v>0.77800000000000002</v>
       </c>
       <c r="J15">
-        <v>1.020408163265306E-2</v>
+        <v>2.2817460317460316E-2</v>
       </c>
       <c r="K15">
-        <v>0.91159052453468681</v>
+        <v>0.92504201680672304</v>
       </c>
       <c r="L15">
-        <v>9.9160000000000004</v>
+        <v>10.287000000000001</v>
       </c>
       <c r="M15">
-        <v>100.98</v>
+        <v>101.05500000000001</v>
       </c>
       <c r="N15">
-        <v>0.77700000000000002</v>
+        <v>0.83899999999999997</v>
       </c>
       <c r="O15">
-        <v>0.77200000000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.82599999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10</v>
       </c>
@@ -1201,46 +1201,46 @@
         <v>5</v>
       </c>
       <c r="C16">
-        <v>1.9221050140253302E-2</v>
+        <v>1.9397400945652173E-2</v>
       </c>
       <c r="D16">
-        <v>0.92002032132667699</v>
+        <v>0.91791810785273653</v>
       </c>
       <c r="E16">
-        <v>8.9209999999999994</v>
+        <v>8.9640000000000004</v>
       </c>
       <c r="F16">
-        <v>110.021</v>
+        <v>109.84699999999999</v>
       </c>
       <c r="G16">
-        <v>7.6050000000000004</v>
+        <v>7.4870000000000001</v>
       </c>
       <c r="H16">
-        <v>1.0549999999999999</v>
+        <v>1.0429999999999999</v>
       </c>
       <c r="I16">
-        <v>1.105</v>
+        <v>1.0309999999999999</v>
       </c>
       <c r="J16">
-        <v>1.2415349887133182E-2</v>
+        <v>2.1920668058455117E-2</v>
       </c>
       <c r="K16">
-        <v>0.91903435468895078</v>
+        <v>0.90912999494183111</v>
       </c>
       <c r="L16">
-        <v>10.021000000000001</v>
+        <v>9.8469999999999995</v>
       </c>
       <c r="M16">
-        <v>101.562</v>
+        <v>101.35899999999999</v>
       </c>
       <c r="N16">
-        <v>1.21</v>
+        <v>1.052</v>
       </c>
       <c r="O16">
-        <v>1.2030000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.0409999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10</v>
       </c>
@@ -1248,43 +1248,43 @@
         <v>10</v>
       </c>
       <c r="C17">
-        <v>1.8924574561296974E-2</v>
+        <v>1.9981952837726549E-2</v>
       </c>
       <c r="D17">
-        <v>0.91574621230687003</v>
+        <v>0.92110386358641283</v>
       </c>
       <c r="E17">
-        <v>9.1300000000000008</v>
+        <v>8.9640000000000004</v>
       </c>
       <c r="F17">
-        <v>110.117</v>
+        <v>109.988</v>
       </c>
       <c r="G17">
-        <v>7.726</v>
+        <v>7.5529999999999999</v>
       </c>
       <c r="H17">
-        <v>1.7969999999999999</v>
+        <v>1.768</v>
       </c>
       <c r="I17">
-        <v>1.9159999999999999</v>
+        <v>1.8260000000000001</v>
       </c>
       <c r="J17">
-        <v>2.5584795321637425E-2</v>
+        <v>1.7925247902364605E-2</v>
       </c>
       <c r="K17">
-        <v>0.90232241223776877</v>
+        <v>0.90548344777535861</v>
       </c>
       <c r="L17">
-        <v>10.117000000000001</v>
+        <v>9.9879999999999995</v>
       </c>
       <c r="M17">
-        <v>102.352</v>
+        <v>102.40600000000001</v>
       </c>
       <c r="N17">
-        <v>1.7829999999999999</v>
+        <v>1.8120000000000001</v>
       </c>
       <c r="O17">
-        <v>1.7689999999999999</v>
+        <v>1.8009999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1293,29 +1293,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28570E15-084B-485C-BB33-408E0188DA61}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DBE3D6E-8BFF-4414-8CE5-827EF1CA9108}">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1356,7 +1355,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>22.981961046756272</v>
       </c>

</xml_diff>